<commit_message>
Analysis for email feb16
</commit_message>
<xml_diff>
--- a/Tables/decomposition_main_te.xlsx
+++ b/Tables/decomposition_main_te.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BB669E-C469-4A9A-98F3-CD255BCBD60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334517EA-DE64-4566-AE8E-7DB6851F7BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-10695" windowWidth="29040" windowHeight="15720" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Observations</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Cost of losing pawn (APR)</t>
+  </si>
+  <si>
+    <t>Control Mean</t>
+  </si>
+  <si>
+    <t>Recovery</t>
   </si>
 </sst>
 </file>
@@ -167,9 +173,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,6 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,37 +245,113 @@
           <cell r="K2" t="str">
             <v>(10)</v>
           </cell>
+          <cell r="L2" t="str">
+            <v>(11)</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>-405.3***</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>166.7*</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>28.4***</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>-109.3***</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>-491.1***</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>0.12***</v>
+          </cell>
+          <cell r="H5" t="str">
+            <v>-39.8***</v>
+          </cell>
+          <cell r="I5" t="str">
+            <v>9.33***</v>
+          </cell>
+          <cell r="J5" t="str">
+            <v>2.43***</v>
+          </cell>
+          <cell r="K5" t="str">
+            <v>-11.1***</v>
+          </cell>
+          <cell r="L5" t="str">
+            <v>-40.4***</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>(139.1)</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>(87.5)</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>(1.09)</v>
+          </cell>
+          <cell r="E6" t="str">
+            <v>(28.3)</v>
+          </cell>
+          <cell r="F6" t="str">
+            <v>(101.0)</v>
+          </cell>
+          <cell r="G6" t="str">
+            <v>(0.022)</v>
+          </cell>
+          <cell r="H6" t="str">
+            <v>(6.41)</v>
+          </cell>
+          <cell r="I6" t="str">
+            <v>(2.65)</v>
+          </cell>
+          <cell r="J6" t="str">
+            <v>(0.11)</v>
+          </cell>
+          <cell r="K6" t="str">
+            <v>(1.88)</v>
+          </cell>
+          <cell r="L6" t="str">
+            <v>(6.99)</v>
+          </cell>
         </row>
         <row r="8">
           <cell r="B8" t="str">
-            <v>-405.4***</v>
+            <v>-155.0</v>
           </cell>
           <cell r="C8" t="str">
-            <v>166.8*</v>
+            <v>-84.8</v>
           </cell>
           <cell r="D8" t="str">
-            <v>28.4***</v>
+            <v>1.25***</v>
           </cell>
           <cell r="E8" t="str">
-            <v>-109.5***</v>
+            <v>-28.6</v>
           </cell>
           <cell r="F8" t="str">
-            <v>-491.1***</v>
+            <v>-42.8</v>
           </cell>
           <cell r="G8" t="str">
-            <v>-39.8***</v>
+            <v>0.0021</v>
           </cell>
           <cell r="H8" t="str">
-            <v>9.36***</v>
+            <v>1.46</v>
           </cell>
           <cell r="I8" t="str">
-            <v>2.43***</v>
+            <v>0.90</v>
           </cell>
           <cell r="J8" t="str">
-            <v>-11.1***</v>
+            <v>0.18***</v>
           </cell>
           <cell r="K8" t="str">
-            <v>-40.5***</v>
+            <v>0.42</v>
+          </cell>
+          <cell r="L8" t="str">
+            <v>-0.038</v>
           </cell>
         </row>
         <row r="9">
@@ -279,200 +359,142 @@
             <v/>
           </cell>
           <cell r="B9" t="str">
-            <v>(139.2)</v>
+            <v>(135.5)</v>
           </cell>
           <cell r="C9" t="str">
-            <v>(87.6)</v>
+            <v>(80.9)</v>
           </cell>
           <cell r="D9" t="str">
-            <v>(1.09)</v>
+            <v>(0.39)</v>
           </cell>
           <cell r="E9" t="str">
-            <v>(28.4)</v>
+            <v>(31.1)</v>
           </cell>
           <cell r="F9" t="str">
-            <v>(101.0)</v>
+            <v>(98.4)</v>
           </cell>
           <cell r="G9" t="str">
-            <v>(6.39)</v>
+            <v>(0.019)</v>
           </cell>
           <cell r="H9" t="str">
-            <v>(2.65)</v>
+            <v>(6.41)</v>
           </cell>
           <cell r="I9" t="str">
-            <v>(0.11)</v>
+            <v>(2.28)</v>
           </cell>
           <cell r="J9" t="str">
-            <v>(1.88)</v>
+            <v>(0.049)</v>
           </cell>
           <cell r="K9" t="str">
-            <v>(6.99)</v>
+            <v>(2.05)</v>
+          </cell>
+          <cell r="L9" t="str">
+            <v>(6.17)</v>
           </cell>
         </row>
         <row r="11">
           <cell r="B11" t="str">
-            <v>-155.3</v>
+            <v>8521</v>
           </cell>
           <cell r="C11" t="str">
-            <v>-84.6</v>
+            <v>8521</v>
           </cell>
           <cell r="D11" t="str">
-            <v>1.25***</v>
+            <v>8521</v>
           </cell>
           <cell r="E11" t="str">
-            <v>-29.1</v>
+            <v>8521</v>
           </cell>
           <cell r="F11" t="str">
-            <v>-42.8</v>
+            <v>8521</v>
           </cell>
           <cell r="G11" t="str">
-            <v>1.62</v>
+            <v>8521</v>
           </cell>
           <cell r="H11" t="str">
-            <v>1.07</v>
+            <v>8521</v>
           </cell>
           <cell r="I11" t="str">
-            <v>0.18***</v>
+            <v>8521</v>
           </cell>
           <cell r="J11" t="str">
-            <v>0.37</v>
+            <v>8521</v>
           </cell>
           <cell r="K11" t="str">
-            <v>0.0026</v>
+            <v>8521</v>
+          </cell>
+          <cell r="L11" t="str">
+            <v>8521</v>
           </cell>
         </row>
         <row r="12">
-          <cell r="A12" t="str">
-            <v/>
-          </cell>
           <cell r="B12" t="str">
-            <v>(135.5)</v>
+            <v>0.010</v>
           </cell>
           <cell r="C12" t="str">
-            <v>(81.0)</v>
+            <v>0.010</v>
           </cell>
           <cell r="D12" t="str">
-            <v>(0.39)</v>
+            <v>0.165</v>
           </cell>
           <cell r="E12" t="str">
-            <v>(31.2)</v>
+            <v>0.021</v>
           </cell>
           <cell r="F12" t="str">
-            <v>(98.4)</v>
+            <v>0.014</v>
           </cell>
           <cell r="G12" t="str">
-            <v>(6.40)</v>
+            <v>0.022</v>
           </cell>
           <cell r="H12" t="str">
-            <v>(2.30)</v>
+            <v>0.039</v>
           </cell>
           <cell r="I12" t="str">
-            <v>(0.049)</v>
+            <v>0.017</v>
           </cell>
           <cell r="J12" t="str">
-            <v>(2.05)</v>
+            <v>0.210</v>
           </cell>
           <cell r="K12" t="str">
-            <v>(6.17)</v>
+            <v>0.041</v>
+          </cell>
+          <cell r="L12" t="str">
+            <v>0.029</v>
           </cell>
         </row>
-        <row r="83">
-          <cell r="B83" t="str">
-            <v>8521</v>
-          </cell>
-          <cell r="C83" t="str">
-            <v>8521</v>
-          </cell>
-          <cell r="D83" t="str">
-            <v>8521</v>
-          </cell>
-          <cell r="E83" t="str">
-            <v>8521</v>
-          </cell>
-          <cell r="F83" t="str">
-            <v>8521</v>
-          </cell>
-          <cell r="G83" t="str">
-            <v>8521</v>
-          </cell>
-          <cell r="H83" t="str">
-            <v>8521</v>
-          </cell>
-          <cell r="I83" t="str">
-            <v>8521</v>
-          </cell>
-          <cell r="J83" t="str">
-            <v>8521</v>
-          </cell>
-          <cell r="K83" t="str">
-            <v>8521</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="B84" t="str">
-            <v>0.010</v>
-          </cell>
-          <cell r="C84" t="str">
-            <v>0.010</v>
-          </cell>
-          <cell r="D84" t="str">
-            <v>0.165</v>
-          </cell>
-          <cell r="E84" t="str">
-            <v>0.021</v>
-          </cell>
-          <cell r="F84" t="str">
-            <v>0.014</v>
-          </cell>
-          <cell r="G84" t="str">
-            <v>0.038</v>
-          </cell>
-          <cell r="H84" t="str">
-            <v>0.017</v>
-          </cell>
-          <cell r="I84" t="str">
-            <v>0.210</v>
-          </cell>
-          <cell r="J84" t="str">
-            <v>0.041</v>
-          </cell>
-          <cell r="K84" t="str">
-            <v>0.029</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85" t="str">
-            <v>Control Mean</v>
-          </cell>
-          <cell r="B85" t="str">
-            <v>3295.6</v>
-          </cell>
-          <cell r="C85" t="str">
-            <v>1109.0</v>
-          </cell>
-          <cell r="D85" t="str">
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>3295.4</v>
+          </cell>
+          <cell r="C13" t="str">
+            <v>1109.2</v>
+          </cell>
+          <cell r="D13" t="str">
             <v>0</v>
           </cell>
-          <cell r="E85" t="str">
-            <v>471.6</v>
-          </cell>
-          <cell r="F85" t="str">
+          <cell r="E13" t="str">
+            <v>471.2</v>
+          </cell>
+          <cell r="F13" t="str">
             <v>1715.0</v>
           </cell>
-          <cell r="G85" t="str">
-            <v/>
-          </cell>
-          <cell r="H85" t="str">
-            <v/>
-          </cell>
-          <cell r="I85" t="str">
-            <v/>
-          </cell>
-          <cell r="J85" t="str">
-            <v/>
-          </cell>
-          <cell r="K85" t="str">
-            <v/>
+          <cell r="G13" t="str">
+            <v>0.44</v>
+          </cell>
+          <cell r="H13" t="str">
+            <v>248.7</v>
+          </cell>
+          <cell r="I13" t="str">
+            <v>47.1</v>
+          </cell>
+          <cell r="J13" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="K13" t="str">
+            <v>38.0</v>
+          </cell>
+          <cell r="L13" t="str">
+            <v>163.5</v>
           </cell>
         </row>
       </sheetData>
@@ -778,23 +800,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FE739-9E07-4309-AA70-62919A677514}">
-  <dimension ref="A2:K22"/>
+  <dimension ref="A2:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F21"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="22.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -811,234 +834,261 @@
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="str">
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="str">
         <f>[1]decomposition_main_te!A2</f>
         <v/>
       </c>
-      <c r="B3" s="6" t="str">
+      <c r="B3" s="5" t="str">
         <f>[1]decomposition_main_te!B2</f>
         <v>(1)</v>
       </c>
-      <c r="C3" s="6" t="str">
+      <c r="C3" s="5" t="str">
         <f>[1]decomposition_main_te!C2</f>
         <v>(2)</v>
       </c>
-      <c r="D3" s="6" t="str">
+      <c r="D3" s="5" t="str">
         <f>[1]decomposition_main_te!D2</f>
         <v>(3)</v>
       </c>
-      <c r="E3" s="6" t="str">
+      <c r="E3" s="5" t="str">
         <f>[1]decomposition_main_te!E2</f>
         <v>(4)</v>
       </c>
-      <c r="F3" s="6" t="str">
+      <c r="F3" s="5" t="str">
         <f>[1]decomposition_main_te!F2</f>
         <v>(5)</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="5" t="str">
+        <f>[1]decomposition_main_te!G2</f>
+        <v>(6)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="str">
-        <f>[1]decomposition_main_te!B8</f>
-        <v>-405.4***</v>
+        <f>[1]decomposition_main_te!B5</f>
+        <v>-405.3***</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>[1]decomposition_main_te!C8</f>
-        <v>166.8*</v>
+        <f>[1]decomposition_main_te!C5</f>
+        <v>166.7*</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f>[1]decomposition_main_te!D8</f>
+        <f>[1]decomposition_main_te!D5</f>
         <v>28.4***</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f>[1]decomposition_main_te!E8</f>
-        <v>-109.5***</v>
+        <f>[1]decomposition_main_te!E5</f>
+        <v>-109.3***</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>[1]decomposition_main_te!F8</f>
+        <f>[1]decomposition_main_te!F5</f>
         <v>-491.1***</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G4" s="1" t="str">
+        <f>[1]decomposition_main_te!G5</f>
+        <v>0.12***</v>
+      </c>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>[1]decomposition_main_te!A9</f>
         <v/>
       </c>
       <c r="B5" s="1" t="str">
-        <f>[1]decomposition_main_te!B9</f>
-        <v>(139.2)</v>
+        <f>[1]decomposition_main_te!B6</f>
+        <v>(139.1)</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f>[1]decomposition_main_te!C9</f>
-        <v>(87.6)</v>
+        <f>[1]decomposition_main_te!C6</f>
+        <v>(87.5)</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f>[1]decomposition_main_te!D9</f>
+        <f>[1]decomposition_main_te!D6</f>
         <v>(1.09)</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f>[1]decomposition_main_te!E9</f>
-        <v>(28.4)</v>
+        <f>[1]decomposition_main_te!E6</f>
+        <v>(28.3)</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>[1]decomposition_main_te!F9</f>
+        <f>[1]decomposition_main_te!F6</f>
         <v>(101.0)</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G5" s="1" t="str">
+        <f>[1]decomposition_main_te!G6</f>
+        <v>(0.022)</v>
+      </c>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="str">
+        <f>[1]decomposition_main_te!B8</f>
+        <v>-155.0</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f>[1]decomposition_main_te!C8</f>
+        <v>-84.8</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>[1]decomposition_main_te!D8</f>
+        <v>1.25***</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f>[1]decomposition_main_te!E8</f>
+        <v>-28.6</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f>[1]decomposition_main_te!F8</f>
+        <v>-42.8</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f>[1]decomposition_main_te!G8</f>
+        <v>0.0021</v>
+      </c>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="str">
+        <f>[1]decomposition_main_te!B9</f>
+        <v>(135.5)</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>[1]decomposition_main_te!C9</f>
+        <v>(80.9)</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>[1]decomposition_main_te!D9</f>
+        <v>(0.39)</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f>[1]decomposition_main_te!E9</f>
+        <v>(31.1)</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f>[1]decomposition_main_te!F9</f>
+        <v>(98.4)</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f>[1]decomposition_main_te!G9</f>
+        <v>(0.019)</v>
+      </c>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="9" t="str">
         <f>[1]decomposition_main_te!B11</f>
-        <v>-155.3</v>
-      </c>
-      <c r="C6" s="1" t="str">
+        <v>8521</v>
+      </c>
+      <c r="C9" s="9" t="str">
         <f>[1]decomposition_main_te!C11</f>
-        <v>-84.6</v>
-      </c>
-      <c r="D6" s="1" t="str">
+        <v>8521</v>
+      </c>
+      <c r="D9" s="9" t="str">
         <f>[1]decomposition_main_te!D11</f>
-        <v>1.25***</v>
-      </c>
-      <c r="E6" s="1" t="str">
+        <v>8521</v>
+      </c>
+      <c r="E9" s="9" t="str">
         <f>[1]decomposition_main_te!E11</f>
-        <v>-29.1</v>
-      </c>
-      <c r="F6" s="1" t="str">
+        <v>8521</v>
+      </c>
+      <c r="F9" s="9" t="str">
         <f>[1]decomposition_main_te!F11</f>
-        <v>-42.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="str">
-        <f>[1]decomposition_main_te!A12</f>
-        <v/>
-      </c>
-      <c r="B7" s="1" t="str">
-        <f>[1]decomposition_main_te!B12</f>
-        <v>(135.5)</v>
-      </c>
-      <c r="C7" s="1" t="str">
-        <f>[1]decomposition_main_te!C12</f>
-        <v>(81.0)</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f>[1]decomposition_main_te!D12</f>
-        <v>(0.39)</v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f>[1]decomposition_main_te!E12</f>
-        <v>(31.2)</v>
-      </c>
-      <c r="F7" s="1" t="str">
-        <f>[1]decomposition_main_te!F12</f>
-        <v>(98.4)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="10" t="str">
-        <f>[1]decomposition_main_te!B83</f>
         <v>8521</v>
       </c>
-      <c r="C9" s="10" t="str">
-        <f>[1]decomposition_main_te!C83</f>
+      <c r="G9" s="9" t="str">
+        <f>[1]decomposition_main_te!G11</f>
         <v>8521</v>
       </c>
-      <c r="D9" s="10" t="str">
-        <f>[1]decomposition_main_te!D83</f>
-        <v>8521</v>
-      </c>
-      <c r="E9" s="10" t="str">
-        <f>[1]decomposition_main_te!E83</f>
-        <v>8521</v>
-      </c>
-      <c r="F9" s="10" t="str">
-        <f>[1]decomposition_main_te!F83</f>
-        <v>8521</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="1" t="str">
-        <f>[1]decomposition_main_te!B84</f>
+        <f>[1]decomposition_main_te!B12</f>
         <v>0.010</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f>[1]decomposition_main_te!C84</f>
+        <f>[1]decomposition_main_te!C12</f>
         <v>0.010</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f>[1]decomposition_main_te!D84</f>
+        <f>[1]decomposition_main_te!D12</f>
         <v>0.165</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f>[1]decomposition_main_te!E84</f>
+        <f>[1]decomposition_main_te!E12</f>
         <v>0.021</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>[1]decomposition_main_te!F84</f>
+        <f>[1]decomposition_main_te!F12</f>
         <v>0.014</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7" t="str">
-        <f>[1]decomposition_main_te!A85</f>
-        <v>Control Mean</v>
-      </c>
-      <c r="B11" s="8" t="str">
-        <f>[1]decomposition_main_te!B85</f>
-        <v>3295.6</v>
-      </c>
-      <c r="C11" s="8" t="str">
-        <f>[1]decomposition_main_te!C85</f>
-        <v>1109.0</v>
-      </c>
-      <c r="D11" s="8" t="str">
-        <f>[1]decomposition_main_te!D85</f>
+      <c r="G10" s="1" t="str">
+        <f>[1]decomposition_main_te!G12</f>
+        <v>0.022</v>
+      </c>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="7" t="str">
+        <f>[1]decomposition_main_te!B13</f>
+        <v>3295.4</v>
+      </c>
+      <c r="C11" s="7" t="str">
+        <f>[1]decomposition_main_te!C13</f>
+        <v>1109.2</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f>[1]decomposition_main_te!D13</f>
         <v>0</v>
       </c>
-      <c r="E11" s="8" t="str">
-        <f>[1]decomposition_main_te!E85</f>
-        <v>471.6</v>
-      </c>
-      <c r="F11" s="8" t="str">
-        <f>[1]decomposition_main_te!F85</f>
+      <c r="E11" s="7" t="str">
+        <f>[1]decomposition_main_te!E13</f>
+        <v>471.2</v>
+      </c>
+      <c r="F11" s="7" t="str">
+        <f>[1]decomposition_main_te!F13</f>
         <v>1715.0</v>
       </c>
-      <c r="G11" s="1" t="str">
-        <f>[1]decomposition_main_te!G85</f>
-        <v/>
-      </c>
-      <c r="H11" t="str">
-        <f>[1]decomposition_main_te!H85</f>
-        <v/>
-      </c>
-      <c r="I11" t="str">
-        <f>[1]decomposition_main_te!I85</f>
-        <v/>
-      </c>
-      <c r="J11" t="str">
-        <f>[1]decomposition_main_te!J85</f>
-        <v/>
-      </c>
-      <c r="K11" t="str">
-        <f>[1]decomposition_main_te!K85</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G11" s="7" t="str">
+        <f>[1]decomposition_main_te!G13</f>
+        <v>0.44</v>
+      </c>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
         <v>8</v>
@@ -1056,76 +1106,76 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6" t="str">
-        <f>[1]decomposition_main_te!G2</f>
-        <v>(6)</v>
-      </c>
-      <c r="C14" s="6" t="str">
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="str">
         <f>[1]decomposition_main_te!H2</f>
         <v>(7)</v>
       </c>
-      <c r="D14" s="6" t="str">
+      <c r="C14" s="5" t="str">
         <f>[1]decomposition_main_te!I2</f>
         <v>(8)</v>
       </c>
-      <c r="E14" s="6" t="str">
+      <c r="D14" s="5" t="str">
         <f>[1]decomposition_main_te!J2</f>
         <v>(9)</v>
       </c>
-      <c r="F14" s="6" t="str">
+      <c r="E14" s="5" t="str">
         <f>[1]decomposition_main_te!K2</f>
         <v>(10)</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="5" t="str">
+        <f>[1]decomposition_main_te!L2</f>
+        <v>(11)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f>[1]decomposition_main_te!G8</f>
+        <f>[1]decomposition_main_te!H5</f>
         <v>-39.8***</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f>[1]decomposition_main_te!H8</f>
-        <v>9.36***</v>
+        <f>[1]decomposition_main_te!I5</f>
+        <v>9.33***</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f>[1]decomposition_main_te!I8</f>
+        <f>[1]decomposition_main_te!J5</f>
         <v>2.43***</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f>[1]decomposition_main_te!J8</f>
+        <f>[1]decomposition_main_te!K5</f>
         <v>-11.1***</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>[1]decomposition_main_te!K8</f>
-        <v>-40.5***</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+        <f>[1]decomposition_main_te!L5</f>
+        <v>-40.4***</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f>[1]decomposition_main_te!G9</f>
-        <v>(6.39)</v>
+        <f>[1]decomposition_main_te!H6</f>
+        <v>(6.41)</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>[1]decomposition_main_te!H9</f>
+        <f>[1]decomposition_main_te!I6</f>
         <v>(2.65)</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f>[1]decomposition_main_te!I9</f>
+        <f>[1]decomposition_main_te!J6</f>
         <v>(0.11)</v>
       </c>
       <c r="E16" s="1" t="str">
-        <f>[1]decomposition_main_te!J9</f>
+        <f>[1]decomposition_main_te!K6</f>
         <v>(1.88)</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>[1]decomposition_main_te!K9</f>
+        <f>[1]decomposition_main_te!L6</f>
         <v>(6.99)</v>
       </c>
     </row>
@@ -1134,24 +1184,24 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="str">
-        <f>[1]decomposition_main_te!G11</f>
-        <v>1.62</v>
+        <f>[1]decomposition_main_te!H8</f>
+        <v>1.46</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>[1]decomposition_main_te!H11</f>
-        <v>1.07</v>
+        <f>[1]decomposition_main_te!I8</f>
+        <v>0.90</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f>[1]decomposition_main_te!I11</f>
+        <f>[1]decomposition_main_te!J8</f>
         <v>0.18***</v>
       </c>
       <c r="E17" s="1" t="str">
-        <f>[1]decomposition_main_te!J11</f>
-        <v>0.37</v>
+        <f>[1]decomposition_main_te!K8</f>
+        <v>0.42</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>[1]decomposition_main_te!K11</f>
-        <v>0.0026</v>
+        <f>[1]decomposition_main_te!L8</f>
+        <v>-0.038</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1159,77 +1209,102 @@
         <v>12</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f>[1]decomposition_main_te!G12</f>
-        <v>(6.40)</v>
+        <f>[1]decomposition_main_te!H9</f>
+        <v>(6.41)</v>
       </c>
       <c r="C18" s="1" t="str">
+        <f>[1]decomposition_main_te!I9</f>
+        <v>(2.28)</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f>[1]decomposition_main_te!J9</f>
+        <v>(0.049)</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f>[1]decomposition_main_te!K9</f>
+        <v>(2.05)</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f>[1]decomposition_main_te!L9</f>
+        <v>(6.17)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="9" t="str">
+        <f>[1]decomposition_main_te!H11</f>
+        <v>8521</v>
+      </c>
+      <c r="C20" s="9" t="str">
+        <f>[1]decomposition_main_te!I11</f>
+        <v>8521</v>
+      </c>
+      <c r="D20" s="9" t="str">
+        <f>[1]decomposition_main_te!J11</f>
+        <v>8521</v>
+      </c>
+      <c r="E20" s="9" t="str">
+        <f>[1]decomposition_main_te!K11</f>
+        <v>8521</v>
+      </c>
+      <c r="F20" s="9" t="str">
+        <f>[1]decomposition_main_te!L11</f>
+        <v>8521</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="str">
         <f>[1]decomposition_main_te!H12</f>
-        <v>(2.30)</v>
-      </c>
-      <c r="D18" s="1" t="str">
+        <v>0.039</v>
+      </c>
+      <c r="C21" s="1" t="str">
         <f>[1]decomposition_main_te!I12</f>
-        <v>(0.049)</v>
-      </c>
-      <c r="E18" s="1" t="str">
+        <v>0.017</v>
+      </c>
+      <c r="D21" s="1" t="str">
         <f>[1]decomposition_main_te!J12</f>
-        <v>(2.05)</v>
-      </c>
-      <c r="F18" s="1" t="str">
+        <v>0.210</v>
+      </c>
+      <c r="E21" s="1" t="str">
         <f>[1]decomposition_main_te!K12</f>
-        <v>(6.17)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+        <v>0.041</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f>[1]decomposition_main_te!L12</f>
+        <v>0.029</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="7" t="str">
+        <f>[1]decomposition_main_te!H13</f>
+        <v>248.7</v>
+      </c>
+      <c r="C22" s="7" t="str">
+        <f>[1]decomposition_main_te!I13</f>
+        <v>47.1</v>
+      </c>
+      <c r="D22" s="7" t="str">
+        <f>[1]decomposition_main_te!J13</f>
         <v>0</v>
       </c>
-      <c r="B20" s="10" t="str">
-        <f>[1]decomposition_main_te!G83</f>
-        <v>8521</v>
-      </c>
-      <c r="C20" s="10" t="str">
-        <f>[1]decomposition_main_te!H83</f>
-        <v>8521</v>
-      </c>
-      <c r="D20" s="10" t="str">
-        <f>[1]decomposition_main_te!I83</f>
-        <v>8521</v>
-      </c>
-      <c r="E20" s="10" t="str">
-        <f>[1]decomposition_main_te!J83</f>
-        <v>8521</v>
-      </c>
-      <c r="F20" s="10" t="str">
-        <f>[1]decomposition_main_te!K83</f>
-        <v>8521</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="8" t="str">
-        <f>[1]decomposition_main_te!G84</f>
-        <v>0.038</v>
-      </c>
-      <c r="C21" s="8" t="str">
-        <f>[1]decomposition_main_te!H84</f>
-        <v>0.017</v>
-      </c>
-      <c r="D21" s="8" t="str">
-        <f>[1]decomposition_main_te!I84</f>
-        <v>0.210</v>
-      </c>
-      <c r="E21" s="8" t="str">
-        <f>[1]decomposition_main_te!J84</f>
-        <v>0.041</v>
-      </c>
-      <c r="F21" s="8" t="str">
-        <f>[1]decomposition_main_te!K84</f>
-        <v>0.029</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="E22" s="7" t="str">
+        <f>[1]decomposition_main_te!K13</f>
+        <v>38.0</v>
+      </c>
+      <c r="F22" s="7" t="str">
+        <f>[1]decomposition_main_te!L13</f>
+        <v>163.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refinement of ML exercises
</commit_message>
<xml_diff>
--- a/Tables/decomposition_main_te.xlsx
+++ b/Tables/decomposition_main_te.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71296FF-EF4D-42E4-BAEA-A7AF8EF3143E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B2225A-33E7-41F8-8190-BF948014BECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17370" yWindow="-13530" windowWidth="19185" windowHeight="11265" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11175" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
   </bookViews>
   <sheets>
     <sheet name="decomposition_main_te" sheetId="1" r:id="rId1"/>
@@ -246,7 +246,7 @@
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>-383.2***</v>
+            <v>-380.0***</v>
           </cell>
           <cell r="C5" t="str">
             <v>-159.5***</v>
@@ -255,13 +255,13 @@
             <v>32.0***</v>
           </cell>
           <cell r="E5" t="str">
-            <v>-255.7**</v>
+            <v>-252.5**</v>
           </cell>
           <cell r="F5" t="str">
-            <v>-0.084</v>
+            <v>0.16</v>
           </cell>
           <cell r="G5" t="str">
-            <v>-0.34***</v>
+            <v>-0.33***</v>
           </cell>
           <cell r="H5" t="str">
             <v>-0.087***</v>
@@ -270,7 +270,7 @@
             <v>0.015***</v>
           </cell>
           <cell r="J5" t="str">
-            <v>-0.20***</v>
+            <v>-0.19***</v>
           </cell>
           <cell r="K5" t="str">
             <v>0.0013</v>
@@ -278,7 +278,7 @@
         </row>
         <row r="6">
           <cell r="B6" t="str">
-            <v>(112.0)</v>
+            <v>(112.1)</v>
           </cell>
           <cell r="C6" t="str">
             <v>(35.2)</v>
@@ -287,13 +287,13 @@
             <v>(1.43)</v>
           </cell>
           <cell r="E6" t="str">
-            <v>(105.1)</v>
+            <v>(105.2)</v>
           </cell>
           <cell r="F6" t="str">
-            <v>(2.79)</v>
+            <v>(2.76)</v>
           </cell>
           <cell r="G6" t="str">
-            <v>(0.080)</v>
+            <v>(0.081)</v>
           </cell>
           <cell r="H6" t="str">
             <v>(0.016)</v>
@@ -310,7 +310,7 @@
         </row>
         <row r="8">
           <cell r="B8" t="str">
-            <v>-91.2</v>
+            <v>-86.4</v>
           </cell>
           <cell r="C8" t="str">
             <v>-32.1</v>
@@ -319,13 +319,13 @@
             <v>1.28**</v>
           </cell>
           <cell r="E8" t="str">
-            <v>-60.4</v>
+            <v>-55.6</v>
           </cell>
           <cell r="F8" t="str">
-            <v>-2.98</v>
+            <v>-2.25</v>
           </cell>
           <cell r="G8" t="str">
-            <v>-0.10</v>
+            <v>-0.098</v>
           </cell>
           <cell r="H8" t="str">
             <v>0.0071</v>
@@ -334,10 +334,10 @@
             <v>0.00099***</v>
           </cell>
           <cell r="J8" t="str">
-            <v>-0.074</v>
+            <v>-0.072</v>
           </cell>
           <cell r="K8" t="str">
-            <v>-0.0011</v>
+            <v>-0.0010</v>
           </cell>
         </row>
         <row r="9">
@@ -345,7 +345,7 @@
             <v/>
           </cell>
           <cell r="B9" t="str">
-            <v>(114.1)</v>
+            <v>(114.3)</v>
           </cell>
           <cell r="C9" t="str">
             <v>(36.9)</v>
@@ -354,13 +354,13 @@
             <v>(0.54)</v>
           </cell>
           <cell r="E9" t="str">
-            <v>(108.8)</v>
+            <v>(109.0)</v>
           </cell>
           <cell r="F9" t="str">
-            <v>(2.06)</v>
+            <v>(2.08)</v>
           </cell>
           <cell r="G9" t="str">
-            <v>(0.072)</v>
+            <v>(0.073)</v>
           </cell>
           <cell r="H9" t="str">
             <v>(0.017)</v>
@@ -424,7 +424,7 @@
             <v>0.003</v>
           </cell>
           <cell r="G12" t="str">
-            <v>0.013</v>
+            <v>0.012</v>
           </cell>
           <cell r="H12" t="str">
             <v>0.063</v>
@@ -433,7 +433,7 @@
             <v>0.268</v>
           </cell>
           <cell r="J12" t="str">
-            <v>0.016</v>
+            <v>0.015</v>
           </cell>
           <cell r="K12" t="str">
             <v>0.005</v>
@@ -441,7 +441,7 @@
         </row>
         <row r="13">
           <cell r="B13" t="str">
-            <v>1851.0</v>
+            <v>1847.7</v>
           </cell>
           <cell r="C13" t="str">
             <v>545.9</v>
@@ -450,10 +450,10 @@
             <v>0</v>
           </cell>
           <cell r="E13" t="str">
-            <v>1305.1</v>
+            <v>1301.8</v>
           </cell>
           <cell r="F13" t="str">
-            <v>5.26</v>
+            <v>4.99</v>
           </cell>
           <cell r="G13" t="str">
             <v>1.83</v>
@@ -465,7 +465,7 @@
             <v>0</v>
           </cell>
           <cell r="J13" t="str">
-            <v>1.38</v>
+            <v>1.37</v>
           </cell>
           <cell r="K13" t="str">
             <v>0.0030</v>
@@ -776,21 +776,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FE739-9E07-4309-AA70-62919A677514}">
   <dimension ref="A2:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F22" sqref="A2:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -808,7 +808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="str">
         <f>[1]decomposition_main_te!A2</f>
         <v/>
@@ -834,13 +834,13 @@
         <v>(5)</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>[1]decomposition_main_te!B5</f>
-        <v>-383.2***</v>
+        <v>-380.0***</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>[1]decomposition_main_te!C5</f>
@@ -852,22 +852,22 @@
       </c>
       <c r="E4" s="1" t="str">
         <f>[1]decomposition_main_te!E5</f>
-        <v>-255.7**</v>
+        <v>-252.5**</v>
       </c>
       <c r="F4" s="1" t="str">
         <f>[1]decomposition_main_te!F5</f>
-        <v>-0.084</v>
+        <v>0.16</v>
       </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>[1]decomposition_main_te!A9</f>
         <v/>
       </c>
       <c r="B5" s="1" t="str">
         <f>[1]decomposition_main_te!B6</f>
-        <v>(112.0)</v>
+        <v>(112.1)</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>[1]decomposition_main_te!C6</f>
@@ -879,21 +879,21 @@
       </c>
       <c r="E5" s="1" t="str">
         <f>[1]decomposition_main_te!E6</f>
-        <v>(105.1)</v>
+        <v>(105.2)</v>
       </c>
       <c r="F5" s="1" t="str">
         <f>[1]decomposition_main_te!F6</f>
-        <v>(2.79)</v>
+        <v>(2.76)</v>
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>[1]decomposition_main_te!B8</f>
-        <v>-91.2</v>
+        <v>-86.4</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>[1]decomposition_main_te!C8</f>
@@ -905,18 +905,18 @@
       </c>
       <c r="E6" s="1" t="str">
         <f>[1]decomposition_main_te!E8</f>
-        <v>-60.4</v>
+        <v>-55.6</v>
       </c>
       <c r="F6" s="1" t="str">
         <f>[1]decomposition_main_te!F8</f>
-        <v>-2.98</v>
+        <v>-2.25</v>
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="str">
         <f>[1]decomposition_main_te!B9</f>
-        <v>(114.1)</v>
+        <v>(114.3)</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>[1]decomposition_main_te!C9</f>
@@ -928,18 +928,18 @@
       </c>
       <c r="E7" s="1" t="str">
         <f>[1]decomposition_main_te!E9</f>
-        <v>(108.8)</v>
+        <v>(109.0)</v>
       </c>
       <c r="F7" s="1" t="str">
         <f>[1]decomposition_main_te!F9</f>
-        <v>(2.06)</v>
+        <v>(2.08)</v>
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
@@ -965,7 +965,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -991,13 +991,13 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="str">
         <f>[1]decomposition_main_te!B13</f>
-        <v>1851.0</v>
+        <v>1847.7</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>[1]decomposition_main_te!C13</f>
@@ -1009,15 +1009,15 @@
       </c>
       <c r="E11" s="7" t="str">
         <f>[1]decomposition_main_te!E13</f>
-        <v>1305.1</v>
+        <v>1301.8</v>
       </c>
       <c r="F11" s="7" t="str">
         <f>[1]decomposition_main_te!F13</f>
-        <v>5.26</v>
+        <v>4.99</v>
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1026,7 +1026,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
         <v>7</v>
@@ -1044,7 +1044,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="str">
         <f>[1]decomposition_main_te!G2</f>
@@ -1067,13 +1067,13 @@
         <v>(10)</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>[1]decomposition_main_te!G5</f>
-        <v>-0.34***</v>
+        <v>-0.33***</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>[1]decomposition_main_te!H5</f>
@@ -1085,20 +1085,20 @@
       </c>
       <c r="E15" s="1" t="str">
         <f>[1]decomposition_main_te!J5</f>
-        <v>-0.20***</v>
+        <v>-0.19***</v>
       </c>
       <c r="F15" s="1" t="str">
         <f>[1]decomposition_main_te!K5</f>
         <v>0.0013</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>[1]decomposition_main_te!G6</f>
-        <v>(0.080)</v>
+        <v>(0.081)</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>[1]decomposition_main_te!H6</f>
@@ -1117,13 +1117,13 @@
         <v>(0.0018)</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="1" t="str">
         <f>[1]decomposition_main_te!G8</f>
-        <v>-0.10</v>
+        <v>-0.098</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>[1]decomposition_main_te!H8</f>
@@ -1135,20 +1135,20 @@
       </c>
       <c r="E17" s="1" t="str">
         <f>[1]decomposition_main_te!J8</f>
-        <v>-0.074</v>
+        <v>-0.072</v>
       </c>
       <c r="F17" s="1" t="str">
         <f>[1]decomposition_main_te!K8</f>
-        <v>-0.0011</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-0.0010</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>[1]decomposition_main_te!G9</f>
-        <v>(0.072)</v>
+        <v>(0.073)</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>[1]decomposition_main_te!H9</f>
@@ -1167,10 +1167,10 @@
         <v>(0.0013)</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>0</v>
       </c>
@@ -1195,13 +1195,13 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="1" t="str">
         <f>[1]decomposition_main_te!G12</f>
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>[1]decomposition_main_te!H12</f>
@@ -1213,14 +1213,14 @@
       </c>
       <c r="E21" s="1" t="str">
         <f>[1]decomposition_main_te!J12</f>
-        <v>0.016</v>
+        <v>0.015</v>
       </c>
       <c r="F21" s="1" t="str">
         <f>[1]decomposition_main_te!K12</f>
         <v>0.005</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>10</v>
       </c>
@@ -1238,14 +1238,14 @@
       </c>
       <c r="E22" s="7" t="str">
         <f>[1]decomposition_main_te!J13</f>
-        <v>1.38</v>
+        <v>1.37</v>
       </c>
       <c r="F22" s="7" t="str">
         <f>[1]decomposition_main_te!K13</f>
         <v>0.0030</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove soft arms, edit ss, and main table results
</commit_message>
<xml_diff>
--- a/Tables/decomposition_main_te.xlsx
+++ b/Tables/decomposition_main_te.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2020\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B2225A-33E7-41F8-8190-BF948014BECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFA7D23-D3B3-43D8-BCD3-0C6BD297D3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11175" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
+    <workbookView xWindow="-22125" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
   </bookViews>
   <sheets>
     <sheet name="decomposition_main_te" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Observations</t>
   </si>
@@ -52,31 +52,31 @@
     <t>FC</t>
   </si>
   <si>
-    <t>Fees</t>
-  </si>
-  <si>
-    <t>Interest</t>
-  </si>
-  <si>
-    <t>Cost of losing pawn</t>
-  </si>
-  <si>
     <t>APR</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>R-squared</t>
   </si>
   <si>
     <t>Control Mean</t>
   </si>
   <si>
-    <t>Capital</t>
-  </si>
-  <si>
-    <t>Interest/Loan</t>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Financial Cost</t>
+  </si>
+  <si>
+    <t>Lost pawn value</t>
+  </si>
+  <si>
+    <t>Interest pymnt</t>
+  </si>
+  <si>
+    <t>Fee pymnt</t>
+  </si>
+  <si>
+    <t>Principal pymnt</t>
   </si>
 </sst>
 </file>
@@ -106,17 +106,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -151,8 +140,19 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,11 +178,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -202,8 +210,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="decomposition_main_te"/>
     </sheetNames>
@@ -234,110 +245,74 @@
           <cell r="H2" t="str">
             <v>(7)</v>
           </cell>
-          <cell r="I2" t="str">
-            <v>(8)</v>
-          </cell>
-          <cell r="J2" t="str">
-            <v>(9)</v>
-          </cell>
-          <cell r="K2" t="str">
-            <v>(10)</v>
-          </cell>
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>-380.0***</v>
+            <v>-379.7***</v>
           </cell>
           <cell r="C5" t="str">
-            <v>-159.5***</v>
+            <v>-157.3***</v>
           </cell>
           <cell r="D5" t="str">
-            <v>32.0***</v>
+            <v>32.1***</v>
           </cell>
           <cell r="E5" t="str">
-            <v>-252.5**</v>
+            <v>-0.57</v>
           </cell>
           <cell r="F5" t="str">
-            <v>0.16</v>
+            <v>-254.5**</v>
           </cell>
           <cell r="G5" t="str">
-            <v>-0.33***</v>
+            <v>-0.065***</v>
           </cell>
           <cell r="H5" t="str">
-            <v>-0.087***</v>
-          </cell>
-          <cell r="I5" t="str">
-            <v>0.015***</v>
-          </cell>
-          <cell r="J5" t="str">
-            <v>-0.19***</v>
-          </cell>
-          <cell r="K5" t="str">
-            <v>0.0013</v>
+            <v>-0.34***</v>
           </cell>
         </row>
         <row r="6">
           <cell r="B6" t="str">
-            <v>(112.1)</v>
+            <v>(111.4)</v>
           </cell>
           <cell r="C6" t="str">
-            <v>(35.2)</v>
+            <v>(34.9)</v>
           </cell>
           <cell r="D6" t="str">
             <v>(1.43)</v>
           </cell>
           <cell r="E6" t="str">
-            <v>(105.2)</v>
+            <v>(3.03)</v>
           </cell>
           <cell r="F6" t="str">
-            <v>(2.76)</v>
+            <v>(104.8)</v>
           </cell>
           <cell r="G6" t="str">
-            <v>(0.081)</v>
+            <v>(0.023)</v>
           </cell>
           <cell r="H6" t="str">
-            <v>(0.016)</v>
-          </cell>
-          <cell r="I6" t="str">
-            <v>(0.00054)</v>
-          </cell>
-          <cell r="J6" t="str">
-            <v>(0.073)</v>
-          </cell>
-          <cell r="K6" t="str">
-            <v>(0.0018)</v>
+            <v>(0.080)</v>
           </cell>
         </row>
         <row r="8">
           <cell r="B8" t="str">
-            <v>-86.4</v>
+            <v>-84.9</v>
           </cell>
           <cell r="C8" t="str">
-            <v>-32.1</v>
+            <v>-24.9</v>
           </cell>
           <cell r="D8" t="str">
-            <v>1.28**</v>
+            <v>1.34**</v>
           </cell>
           <cell r="E8" t="str">
-            <v>-55.6</v>
+            <v>-3.98</v>
           </cell>
           <cell r="F8" t="str">
-            <v>-2.25</v>
+            <v>-61.4</v>
           </cell>
           <cell r="G8" t="str">
-            <v>-0.098</v>
+            <v>-0.025</v>
           </cell>
           <cell r="H8" t="str">
-            <v>0.0071</v>
-          </cell>
-          <cell r="I8" t="str">
-            <v>0.00099***</v>
-          </cell>
-          <cell r="J8" t="str">
-            <v>-0.072</v>
-          </cell>
-          <cell r="K8" t="str">
-            <v>-0.0010</v>
+            <v>-0.12</v>
           </cell>
         </row>
         <row r="9">
@@ -345,34 +320,25 @@
             <v/>
           </cell>
           <cell r="B9" t="str">
-            <v>(114.3)</v>
+            <v>(114.6)</v>
           </cell>
           <cell r="C9" t="str">
-            <v>(36.9)</v>
+            <v>(38.4)</v>
           </cell>
           <cell r="D9" t="str">
             <v>(0.54)</v>
           </cell>
           <cell r="E9" t="str">
-            <v>(109.0)</v>
+            <v>(2.47)</v>
           </cell>
           <cell r="F9" t="str">
-            <v>(2.08)</v>
+            <v>(109.2)</v>
           </cell>
           <cell r="G9" t="str">
+            <v>(0.021)</v>
+          </cell>
+          <cell r="H9" t="str">
             <v>(0.073)</v>
-          </cell>
-          <cell r="H9" t="str">
-            <v>(0.017)</v>
-          </cell>
-          <cell r="I9" t="str">
-            <v>(0.00028)</v>
-          </cell>
-          <cell r="J9" t="str">
-            <v>(0.067)</v>
-          </cell>
-          <cell r="K9" t="str">
-            <v>(0.0013)</v>
           </cell>
         </row>
         <row r="11">
@@ -397,51 +363,33 @@
           <cell r="H11" t="str">
             <v>6304</v>
           </cell>
-          <cell r="I11" t="str">
-            <v>6304</v>
-          </cell>
-          <cell r="J11" t="str">
-            <v>6304</v>
-          </cell>
-          <cell r="K11" t="str">
-            <v>6304</v>
-          </cell>
         </row>
         <row r="12">
           <cell r="B12" t="str">
-            <v>0.008</v>
+            <v>0.007</v>
           </cell>
           <cell r="C12" t="str">
-            <v>0.030</v>
+            <v>0.022</v>
           </cell>
           <cell r="D12" t="str">
             <v>0.151</v>
           </cell>
           <cell r="E12" t="str">
-            <v>0.008</v>
+            <v>0.003</v>
           </cell>
           <cell r="F12" t="str">
-            <v>0.003</v>
+            <v>0.007</v>
           </cell>
           <cell r="G12" t="str">
-            <v>0.012</v>
+            <v>0.013</v>
           </cell>
           <cell r="H12" t="str">
-            <v>0.063</v>
-          </cell>
-          <cell r="I12" t="str">
-            <v>0.268</v>
-          </cell>
-          <cell r="J12" t="str">
-            <v>0.015</v>
-          </cell>
-          <cell r="K12" t="str">
-            <v>0.005</v>
+            <v>0.011</v>
           </cell>
         </row>
         <row r="13">
           <cell r="B13" t="str">
-            <v>1847.7</v>
+            <v>1851.0</v>
           </cell>
           <cell r="C13" t="str">
             <v>545.9</v>
@@ -450,25 +398,16 @@
             <v>0</v>
           </cell>
           <cell r="E13" t="str">
-            <v>1301.8</v>
+            <v>5.82</v>
           </cell>
           <cell r="F13" t="str">
-            <v>4.99</v>
+            <v>1305.1</v>
           </cell>
           <cell r="G13" t="str">
-            <v>1.83</v>
+            <v>0.44</v>
           </cell>
           <cell r="H13" t="str">
-            <v>0.30</v>
-          </cell>
-          <cell r="I13" t="str">
-            <v>0</v>
-          </cell>
-          <cell r="J13" t="str">
-            <v>1.37</v>
-          </cell>
-          <cell r="K13" t="str">
-            <v>0.0030</v>
+            <v>1.84</v>
           </cell>
         </row>
       </sheetData>
@@ -774,479 +713,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FE739-9E07-4309-AA70-62919A677514}">
-  <dimension ref="A2:L23"/>
+  <dimension ref="A2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F22" sqref="A2:F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="A2:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="3.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="6"/>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="str">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="str">
         <f>[1]decomposition_main_te!A2</f>
         <v/>
       </c>
-      <c r="B3" s="5" t="str">
+      <c r="B4" s="3" t="str">
         <f>[1]decomposition_main_te!B2</f>
         <v>(1)</v>
       </c>
-      <c r="C3" s="5" t="str">
+      <c r="C4" s="3" t="str">
         <f>[1]decomposition_main_te!C2</f>
         <v>(2)</v>
       </c>
-      <c r="D3" s="5" t="str">
+      <c r="D4" s="3" t="str">
         <f>[1]decomposition_main_te!D2</f>
         <v>(3)</v>
       </c>
-      <c r="E3" s="5" t="str">
+      <c r="E4" s="3" t="str">
         <f>[1]decomposition_main_te!E2</f>
         <v>(4)</v>
       </c>
-      <c r="F3" s="5" t="str">
+      <c r="F4" s="3" t="str">
         <f>[1]decomposition_main_te!F2</f>
         <v>(5)</v>
       </c>
+      <c r="G4" s="3" t="str">
+        <f>[1]decomposition_main_te!G2</f>
+        <v>(6)</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="str">
+        <f>[1]decomposition_main_te!H2</f>
+        <v>(7)</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="str">
+      <c r="B5" s="1" t="str">
         <f>[1]decomposition_main_te!B5</f>
-        <v>-380.0***</v>
-      </c>
-      <c r="C4" s="1" t="str">
+        <v>-379.7***</v>
+      </c>
+      <c r="C5" s="1" t="str">
         <f>[1]decomposition_main_te!C5</f>
-        <v>-159.5***</v>
-      </c>
-      <c r="D4" s="1" t="str">
+        <v>-157.3***</v>
+      </c>
+      <c r="D5" s="1" t="str">
         <f>[1]decomposition_main_te!D5</f>
-        <v>32.0***</v>
-      </c>
-      <c r="E4" s="1" t="str">
+        <v>32.1***</v>
+      </c>
+      <c r="E5" s="1" t="str">
         <f>[1]decomposition_main_te!E5</f>
-        <v>-252.5**</v>
-      </c>
-      <c r="F4" s="1" t="str">
+        <v>-0.57</v>
+      </c>
+      <c r="F5" s="1" t="str">
         <f>[1]decomposition_main_te!F5</f>
-        <v>0.16</v>
-      </c>
-      <c r="L4" s="1"/>
+        <v>-254.5**</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f>[1]decomposition_main_te!G5</f>
+        <v>-0.065***</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>[1]decomposition_main_te!H5</f>
+        <v>-0.34***</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="str">
         <f>[1]decomposition_main_te!A9</f>
         <v/>
       </c>
-      <c r="B5" s="1" t="str">
+      <c r="B6" s="1" t="str">
         <f>[1]decomposition_main_te!B6</f>
-        <v>(112.1)</v>
-      </c>
-      <c r="C5" s="1" t="str">
+        <v>(111.4)</v>
+      </c>
+      <c r="C6" s="1" t="str">
         <f>[1]decomposition_main_te!C6</f>
-        <v>(35.2)</v>
-      </c>
-      <c r="D5" s="1" t="str">
+        <v>(34.9)</v>
+      </c>
+      <c r="D6" s="1" t="str">
         <f>[1]decomposition_main_te!D6</f>
         <v>(1.43)</v>
       </c>
-      <c r="E5" s="1" t="str">
+      <c r="E6" s="1" t="str">
         <f>[1]decomposition_main_te!E6</f>
-        <v>(105.2)</v>
-      </c>
-      <c r="F5" s="1" t="str">
+        <v>(3.03)</v>
+      </c>
+      <c r="F6" s="1" t="str">
         <f>[1]decomposition_main_te!F6</f>
-        <v>(2.76)</v>
-      </c>
-      <c r="L5" s="1"/>
+        <v>(104.8)</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f>[1]decomposition_main_te!G6</f>
+        <v>(0.023)</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>[1]decomposition_main_te!H6</f>
+        <v>(0.080)</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="str">
+      <c r="B7" s="1" t="str">
         <f>[1]decomposition_main_te!B8</f>
-        <v>-86.4</v>
-      </c>
-      <c r="C6" s="1" t="str">
+        <v>-84.9</v>
+      </c>
+      <c r="C7" s="1" t="str">
         <f>[1]decomposition_main_te!C8</f>
-        <v>-32.1</v>
-      </c>
-      <c r="D6" s="1" t="str">
+        <v>-24.9</v>
+      </c>
+      <c r="D7" s="1" t="str">
         <f>[1]decomposition_main_te!D8</f>
-        <v>1.28**</v>
-      </c>
-      <c r="E6" s="1" t="str">
+        <v>1.34**</v>
+      </c>
+      <c r="E7" s="1" t="str">
         <f>[1]decomposition_main_te!E8</f>
-        <v>-55.6</v>
-      </c>
-      <c r="F6" s="1" t="str">
+        <v>-3.98</v>
+      </c>
+      <c r="F7" s="1" t="str">
         <f>[1]decomposition_main_te!F8</f>
-        <v>-2.25</v>
-      </c>
-      <c r="L6" s="1"/>
+        <v>-61.4</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f>[1]decomposition_main_te!G8</f>
+        <v>-0.025</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f>[1]decomposition_main_te!H8</f>
+        <v>-0.12</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="str">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="str">
         <f>[1]decomposition_main_te!B9</f>
-        <v>(114.3)</v>
-      </c>
-      <c r="C7" s="1" t="str">
+        <v>(114.6)</v>
+      </c>
+      <c r="C8" s="1" t="str">
         <f>[1]decomposition_main_te!C9</f>
-        <v>(36.9)</v>
-      </c>
-      <c r="D7" s="1" t="str">
+        <v>(38.4)</v>
+      </c>
+      <c r="D8" s="1" t="str">
         <f>[1]decomposition_main_te!D9</f>
         <v>(0.54)</v>
       </c>
-      <c r="E7" s="1" t="str">
+      <c r="E8" s="1" t="str">
         <f>[1]decomposition_main_te!E9</f>
-        <v>(109.0)</v>
-      </c>
-      <c r="F7" s="1" t="str">
+        <v>(2.47)</v>
+      </c>
+      <c r="F8" s="1" t="str">
         <f>[1]decomposition_main_te!F9</f>
-        <v>(2.08)</v>
-      </c>
-      <c r="L7" s="1"/>
+        <v>(109.2)</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f>[1]decomposition_main_te!G9</f>
+        <v>(0.021)</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f>[1]decomposition_main_te!H9</f>
+        <v>(0.073)</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L8" s="1"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I9" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="9" t="str">
+      <c r="B10" s="7" t="str">
         <f>[1]decomposition_main_te!B11</f>
         <v>6304</v>
       </c>
-      <c r="C9" s="9" t="str">
+      <c r="C10" s="7" t="str">
         <f>[1]decomposition_main_te!C11</f>
         <v>6304</v>
       </c>
-      <c r="D9" s="9" t="str">
+      <c r="D10" s="7" t="str">
         <f>[1]decomposition_main_te!D11</f>
         <v>6304</v>
       </c>
-      <c r="E9" s="9" t="str">
+      <c r="E10" s="7" t="str">
         <f>[1]decomposition_main_te!E11</f>
         <v>6304</v>
       </c>
-      <c r="F9" s="9" t="str">
+      <c r="F10" s="7" t="str">
         <f>[1]decomposition_main_te!F11</f>
         <v>6304</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="G10" s="7" t="str">
+        <f>[1]decomposition_main_te!G11</f>
+        <v>6304</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7" t="str">
+        <f>[1]decomposition_main_te!H11</f>
+        <v>6304</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="str">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="str">
         <f>[1]decomposition_main_te!B12</f>
-        <v>0.008</v>
-      </c>
-      <c r="C10" s="1" t="str">
+        <v>0.007</v>
+      </c>
+      <c r="C11" s="1" t="str">
         <f>[1]decomposition_main_te!C12</f>
-        <v>0.030</v>
-      </c>
-      <c r="D10" s="1" t="str">
+        <v>0.022</v>
+      </c>
+      <c r="D11" s="1" t="str">
         <f>[1]decomposition_main_te!D12</f>
         <v>0.151</v>
       </c>
-      <c r="E10" s="1" t="str">
+      <c r="E11" s="1" t="str">
         <f>[1]decomposition_main_te!E12</f>
-        <v>0.008</v>
-      </c>
-      <c r="F10" s="1" t="str">
+        <v>0.003</v>
+      </c>
+      <c r="F11" s="1" t="str">
         <f>[1]decomposition_main_te!F12</f>
-        <v>0.003</v>
-      </c>
-      <c r="L10" s="1"/>
+        <v>0.007</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f>[1]decomposition_main_te!G12</f>
+        <v>0.013</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f>[1]decomposition_main_te!H12</f>
+        <v>0.011</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="str">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="5" t="str">
         <f>[1]decomposition_main_te!B13</f>
-        <v>1847.7</v>
-      </c>
-      <c r="C11" s="7" t="str">
+        <v>1851.0</v>
+      </c>
+      <c r="C12" s="5" t="str">
         <f>[1]decomposition_main_te!C13</f>
         <v>545.9</v>
       </c>
-      <c r="D11" s="7" t="str">
+      <c r="D12" s="5" t="str">
         <f>[1]decomposition_main_te!D13</f>
         <v>0</v>
       </c>
-      <c r="E11" s="7" t="str">
+      <c r="E12" s="5" t="str">
         <f>[1]decomposition_main_te!E13</f>
-        <v>1301.8</v>
-      </c>
-      <c r="F11" s="7" t="str">
+        <v>5.82</v>
+      </c>
+      <c r="F12" s="5" t="str">
         <f>[1]decomposition_main_te!F13</f>
-        <v>4.99</v>
-      </c>
-      <c r="L11" s="1"/>
+        <v>1305.1</v>
+      </c>
+      <c r="G12" s="5" t="str">
+        <f>[1]decomposition_main_te!G13</f>
+        <v>0.44</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5" t="str">
+        <f>[1]decomposition_main_te!H13</f>
+        <v>1.84</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="str">
-        <f>[1]decomposition_main_te!G2</f>
-        <v>(6)</v>
-      </c>
-      <c r="C14" s="5" t="str">
-        <f>[1]decomposition_main_te!H2</f>
-        <v>(7)</v>
-      </c>
-      <c r="D14" s="5" t="str">
-        <f>[1]decomposition_main_te!I2</f>
-        <v>(8)</v>
-      </c>
-      <c r="E14" s="5" t="str">
-        <f>[1]decomposition_main_te!J2</f>
-        <v>(9)</v>
-      </c>
-      <c r="F14" s="5" t="str">
-        <f>[1]decomposition_main_te!K2</f>
-        <v>(10)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="str">
-        <f>[1]decomposition_main_te!G5</f>
-        <v>-0.33***</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f>[1]decomposition_main_te!H5</f>
-        <v>-0.087***</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f>[1]decomposition_main_te!I5</f>
-        <v>0.015***</v>
-      </c>
-      <c r="E15" s="1" t="str">
-        <f>[1]decomposition_main_te!J5</f>
-        <v>-0.19***</v>
-      </c>
-      <c r="F15" s="1" t="str">
-        <f>[1]decomposition_main_te!K5</f>
-        <v>0.0013</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="str">
-        <f>[1]decomposition_main_te!G6</f>
-        <v>(0.081)</v>
-      </c>
-      <c r="C16" s="1" t="str">
-        <f>[1]decomposition_main_te!H6</f>
-        <v>(0.016)</v>
-      </c>
-      <c r="D16" s="1" t="str">
-        <f>[1]decomposition_main_te!I6</f>
-        <v>(0.00054)</v>
-      </c>
-      <c r="E16" s="1" t="str">
-        <f>[1]decomposition_main_te!J6</f>
-        <v>(0.073)</v>
-      </c>
-      <c r="F16" s="1" t="str">
-        <f>[1]decomposition_main_te!K6</f>
-        <v>(0.0018)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1" t="str">
-        <f>[1]decomposition_main_te!G8</f>
-        <v>-0.098</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f>[1]decomposition_main_te!H8</f>
-        <v>0.0071</v>
-      </c>
-      <c r="D17" s="1" t="str">
-        <f>[1]decomposition_main_te!I8</f>
-        <v>0.00099***</v>
-      </c>
-      <c r="E17" s="1" t="str">
-        <f>[1]decomposition_main_te!J8</f>
-        <v>-0.072</v>
-      </c>
-      <c r="F17" s="1" t="str">
-        <f>[1]decomposition_main_te!K8</f>
-        <v>-0.0010</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1" t="str">
-        <f>[1]decomposition_main_te!G9</f>
-        <v>(0.073)</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f>[1]decomposition_main_te!H9</f>
-        <v>(0.017)</v>
-      </c>
-      <c r="D18" s="1" t="str">
-        <f>[1]decomposition_main_te!I9</f>
-        <v>(0.00028)</v>
-      </c>
-      <c r="E18" s="1" t="str">
-        <f>[1]decomposition_main_te!J9</f>
-        <v>(0.067)</v>
-      </c>
-      <c r="F18" s="1" t="str">
-        <f>[1]decomposition_main_te!K9</f>
-        <v>(0.0013)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="9" t="str">
-        <f>[1]decomposition_main_te!G11</f>
-        <v>6304</v>
-      </c>
-      <c r="C20" s="9" t="str">
-        <f>[1]decomposition_main_te!H11</f>
-        <v>6304</v>
-      </c>
-      <c r="D20" s="9" t="str">
-        <f>[1]decomposition_main_te!I11</f>
-        <v>6304</v>
-      </c>
-      <c r="E20" s="9" t="str">
-        <f>[1]decomposition_main_te!J11</f>
-        <v>6304</v>
-      </c>
-      <c r="F20" s="9" t="str">
-        <f>[1]decomposition_main_te!K11</f>
-        <v>6304</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f>[1]decomposition_main_te!G12</f>
-        <v>0.012</v>
-      </c>
-      <c r="C21" s="1" t="str">
-        <f>[1]decomposition_main_te!H12</f>
-        <v>0.063</v>
-      </c>
-      <c r="D21" s="1" t="str">
-        <f>[1]decomposition_main_te!I12</f>
-        <v>0.268</v>
-      </c>
-      <c r="E21" s="1" t="str">
-        <f>[1]decomposition_main_te!J12</f>
-        <v>0.015</v>
-      </c>
-      <c r="F21" s="1" t="str">
-        <f>[1]decomposition_main_te!K12</f>
-        <v>0.005</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="7" t="str">
-        <f>[1]decomposition_main_te!G13</f>
-        <v>1.83</v>
-      </c>
-      <c r="C22" s="7" t="str">
-        <f>[1]decomposition_main_te!H13</f>
-        <v>0.30</v>
-      </c>
-      <c r="D22" s="7" t="str">
-        <f>[1]decomposition_main_te!I13</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="7" t="str">
-        <f>[1]decomposition_main_te!J13</f>
-        <v>1.37</v>
-      </c>
-      <c r="F22" s="7" t="str">
-        <f>[1]decomposition_main_te!K13</f>
-        <v>0.0030</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bounding censoring te & other results
</commit_message>
<xml_diff>
--- a/Tables/decomposition_main_te.xlsx
+++ b/Tables/decomposition_main_te.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFA7D23-D3B3-43D8-BCD3-0C6BD297D3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0887EE9-5702-4D9E-B357-EEBBF21B4F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22125" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
+    <workbookView xWindow="4240" yWindow="0" windowWidth="12030" windowHeight="11280" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
   </bookViews>
   <sheets>
     <sheet name="decomposition_main_te" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Observations</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Default</t>
   </si>
   <si>
-    <t>Financial Cost</t>
-  </si>
-  <si>
     <t>Lost pawn value</t>
   </si>
   <si>
@@ -76,7 +73,25 @@
     <t>Fee pymnt</t>
   </si>
   <si>
+    <t>\sum_t P^i_{it}</t>
+  </si>
+  <si>
+    <t>\sum_t P^f_{it}</t>
+  </si>
+  <si>
+    <t>Components of FC</t>
+  </si>
+  <si>
     <t>Principal pymnt</t>
+  </si>
+  <si>
+    <t>\mathds{1}(\text{Def}_i)}\times\sum_t P^c_{it}</t>
+  </si>
+  <si>
+    <t>\mathds{1}(\text{Def}_i)</t>
+  </si>
+  <si>
+    <t>\mathds{1}(\text{Def}_i)}\times \text{Appr. Val.}_i</t>
   </si>
 </sst>
 </file>
@@ -100,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -157,11 +172,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,20 +202,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -713,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FE739-9E07-4309-AA70-62919A677514}">
-  <dimension ref="A2:I13"/>
+  <dimension ref="A2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="A2:I12"/>
+      <selection activeCell="I13" sqref="A2:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,320 +748,337 @@
     <col min="5" max="5" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="8" width="3.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="13"/>
-      <c r="B3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="str">
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="str">
         <f>[1]decomposition_main_te!A2</f>
         <v/>
       </c>
-      <c r="B4" s="3" t="str">
+      <c r="B5" s="3" t="str">
         <f>[1]decomposition_main_te!B2</f>
         <v>(1)</v>
       </c>
-      <c r="C4" s="3" t="str">
+      <c r="C5" s="3" t="str">
         <f>[1]decomposition_main_te!C2</f>
         <v>(2)</v>
       </c>
-      <c r="D4" s="3" t="str">
+      <c r="D5" s="3" t="str">
         <f>[1]decomposition_main_te!D2</f>
         <v>(3)</v>
       </c>
-      <c r="E4" s="3" t="str">
+      <c r="E5" s="3" t="str">
         <f>[1]decomposition_main_te!E2</f>
         <v>(4)</v>
       </c>
-      <c r="F4" s="3" t="str">
+      <c r="F5" s="3" t="str">
         <f>[1]decomposition_main_te!F2</f>
         <v>(5)</v>
       </c>
-      <c r="G4" s="3" t="str">
+      <c r="G5" s="3" t="str">
         <f>[1]decomposition_main_te!G2</f>
         <v>(6)</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="str">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="str">
         <f>[1]decomposition_main_te!H2</f>
         <v>(7)</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="str">
+      <c r="B6" s="1" t="str">
         <f>[1]decomposition_main_te!B5</f>
         <v>-379.7***</v>
       </c>
-      <c r="C5" s="1" t="str">
+      <c r="C6" s="1" t="str">
         <f>[1]decomposition_main_te!C5</f>
         <v>-157.3***</v>
       </c>
-      <c r="D5" s="1" t="str">
+      <c r="D6" s="1" t="str">
         <f>[1]decomposition_main_te!D5</f>
         <v>32.1***</v>
       </c>
-      <c r="E5" s="1" t="str">
+      <c r="E6" s="1" t="str">
         <f>[1]decomposition_main_te!E5</f>
         <v>-0.57</v>
       </c>
-      <c r="F5" s="1" t="str">
+      <c r="F6" s="1" t="str">
         <f>[1]decomposition_main_te!F5</f>
         <v>-254.5**</v>
       </c>
-      <c r="G5" s="1" t="str">
+      <c r="G6" s="1" t="str">
         <f>[1]decomposition_main_te!G5</f>
         <v>-0.065***</v>
       </c>
-      <c r="I5" s="1" t="str">
+      <c r="I6" s="1" t="str">
         <f>[1]decomposition_main_te!H5</f>
         <v>-0.34***</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="str">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="str">
         <f>[1]decomposition_main_te!A9</f>
         <v/>
       </c>
-      <c r="B6" s="1" t="str">
+      <c r="B7" s="1" t="str">
         <f>[1]decomposition_main_te!B6</f>
         <v>(111.4)</v>
       </c>
-      <c r="C6" s="1" t="str">
+      <c r="C7" s="1" t="str">
         <f>[1]decomposition_main_te!C6</f>
         <v>(34.9)</v>
       </c>
-      <c r="D6" s="1" t="str">
+      <c r="D7" s="1" t="str">
         <f>[1]decomposition_main_te!D6</f>
         <v>(1.43)</v>
       </c>
-      <c r="E6" s="1" t="str">
+      <c r="E7" s="1" t="str">
         <f>[1]decomposition_main_te!E6</f>
         <v>(3.03)</v>
       </c>
-      <c r="F6" s="1" t="str">
+      <c r="F7" s="1" t="str">
         <f>[1]decomposition_main_te!F6</f>
         <v>(104.8)</v>
       </c>
-      <c r="G6" s="1" t="str">
+      <c r="G7" s="1" t="str">
         <f>[1]decomposition_main_te!G6</f>
         <v>(0.023)</v>
       </c>
-      <c r="I6" s="1" t="str">
+      <c r="I7" s="1" t="str">
         <f>[1]decomposition_main_te!H6</f>
         <v>(0.080)</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="str">
+      <c r="B8" s="1" t="str">
         <f>[1]decomposition_main_te!B8</f>
         <v>-84.9</v>
       </c>
-      <c r="C7" s="1" t="str">
+      <c r="C8" s="1" t="str">
         <f>[1]decomposition_main_te!C8</f>
         <v>-24.9</v>
       </c>
-      <c r="D7" s="1" t="str">
+      <c r="D8" s="1" t="str">
         <f>[1]decomposition_main_te!D8</f>
         <v>1.34**</v>
       </c>
-      <c r="E7" s="1" t="str">
+      <c r="E8" s="1" t="str">
         <f>[1]decomposition_main_te!E8</f>
         <v>-3.98</v>
       </c>
-      <c r="F7" s="1" t="str">
+      <c r="F8" s="1" t="str">
         <f>[1]decomposition_main_te!F8</f>
         <v>-61.4</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="G8" s="1" t="str">
         <f>[1]decomposition_main_te!G8</f>
         <v>-0.025</v>
       </c>
-      <c r="I7" s="1" t="str">
+      <c r="I8" s="1" t="str">
         <f>[1]decomposition_main_te!H8</f>
         <v>-0.12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="str">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="str">
         <f>[1]decomposition_main_te!B9</f>
         <v>(114.6)</v>
       </c>
-      <c r="C8" s="1" t="str">
+      <c r="C9" s="1" t="str">
         <f>[1]decomposition_main_te!C9</f>
         <v>(38.4)</v>
       </c>
-      <c r="D8" s="1" t="str">
+      <c r="D9" s="1" t="str">
         <f>[1]decomposition_main_te!D9</f>
         <v>(0.54)</v>
       </c>
-      <c r="E8" s="1" t="str">
+      <c r="E9" s="1" t="str">
         <f>[1]decomposition_main_te!E9</f>
         <v>(2.47)</v>
       </c>
-      <c r="F8" s="1" t="str">
+      <c r="F9" s="1" t="str">
         <f>[1]decomposition_main_te!F9</f>
         <v>(109.2)</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="G9" s="1" t="str">
         <f>[1]decomposition_main_te!G9</f>
         <v>(0.021)</v>
       </c>
-      <c r="I8" s="1" t="str">
+      <c r="I9" s="1" t="str">
         <f>[1]decomposition_main_te!H9</f>
         <v>(0.073)</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="I9" s="1"/>
-    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="7" t="str">
+      <c r="B11" s="7" t="str">
         <f>[1]decomposition_main_te!B11</f>
         <v>6304</v>
       </c>
-      <c r="C10" s="7" t="str">
+      <c r="C11" s="7" t="str">
         <f>[1]decomposition_main_te!C11</f>
         <v>6304</v>
       </c>
-      <c r="D10" s="7" t="str">
+      <c r="D11" s="7" t="str">
         <f>[1]decomposition_main_te!D11</f>
         <v>6304</v>
       </c>
-      <c r="E10" s="7" t="str">
+      <c r="E11" s="7" t="str">
         <f>[1]decomposition_main_te!E11</f>
         <v>6304</v>
       </c>
-      <c r="F10" s="7" t="str">
+      <c r="F11" s="7" t="str">
         <f>[1]decomposition_main_te!F11</f>
         <v>6304</v>
       </c>
-      <c r="G10" s="7" t="str">
+      <c r="G11" s="7" t="str">
         <f>[1]decomposition_main_te!G11</f>
         <v>6304</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7" t="str">
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="str">
         <f>[1]decomposition_main_te!H11</f>
         <v>6304</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="str">
+      <c r="B12" s="1" t="str">
         <f>[1]decomposition_main_te!B12</f>
         <v>0.007</v>
       </c>
-      <c r="C11" s="1" t="str">
+      <c r="C12" s="1" t="str">
         <f>[1]decomposition_main_te!C12</f>
         <v>0.022</v>
       </c>
-      <c r="D11" s="1" t="str">
+      <c r="D12" s="1" t="str">
         <f>[1]decomposition_main_te!D12</f>
         <v>0.151</v>
       </c>
-      <c r="E11" s="1" t="str">
+      <c r="E12" s="1" t="str">
         <f>[1]decomposition_main_te!E12</f>
         <v>0.003</v>
       </c>
-      <c r="F11" s="1" t="str">
+      <c r="F12" s="1" t="str">
         <f>[1]decomposition_main_te!F12</f>
         <v>0.007</v>
       </c>
-      <c r="G11" s="1" t="str">
+      <c r="G12" s="1" t="str">
         <f>[1]decomposition_main_te!G12</f>
         <v>0.013</v>
       </c>
-      <c r="I11" s="1" t="str">
+      <c r="I12" s="1" t="str">
         <f>[1]decomposition_main_te!H12</f>
         <v>0.011</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5" t="str">
+      <c r="B13" s="5" t="str">
         <f>[1]decomposition_main_te!B13</f>
         <v>1851.0</v>
       </c>
-      <c r="C12" s="5" t="str">
+      <c r="C13" s="5" t="str">
         <f>[1]decomposition_main_te!C13</f>
         <v>545.9</v>
       </c>
-      <c r="D12" s="5" t="str">
+      <c r="D13" s="5" t="str">
         <f>[1]decomposition_main_te!D13</f>
         <v>0</v>
       </c>
-      <c r="E12" s="5" t="str">
+      <c r="E13" s="5" t="str">
         <f>[1]decomposition_main_te!E13</f>
         <v>5.82</v>
       </c>
-      <c r="F12" s="5" t="str">
+      <c r="F13" s="5" t="str">
         <f>[1]decomposition_main_te!F13</f>
         <v>1305.1</v>
       </c>
-      <c r="G12" s="5" t="str">
+      <c r="G13" s="5" t="str">
         <f>[1]decomposition_main_te!G13</f>
         <v>0.44</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5" t="str">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="str">
         <f>[1]decomposition_main_te!H13</f>
         <v>1.84</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Prepare draft for submission
</commit_message>
<xml_diff>
--- a/Tables/decomposition_main_te.xlsx
+++ b/Tables/decomposition_main_te.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A579E14-FC2D-4076-8D66-ECAB439546A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB29A75-538C-4DCD-9520-53E3F0C4F176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18945" yWindow="-12450" windowWidth="21600" windowHeight="11235" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
+    <workbookView xWindow="-24630" yWindow="1875" windowWidth="28800" windowHeight="13335" xr2:uid="{3609313A-5DBD-4B39-A88D-6C774A33806E}"/>
   </bookViews>
   <sheets>
     <sheet name="decomposition_main_te" sheetId="1" r:id="rId1"/>
@@ -79,19 +79,19 @@
     <t>Principal pymnt</t>
   </si>
   <si>
-    <t>$\sum_t P^i_{it}$</t>
-  </si>
-  <si>
-    <t>$\sum_t P^f_{it}$</t>
-  </si>
-  <si>
-    <t>$\mathds{1}(\text{Def}_i)}\times\sum_t P^c_{it}$</t>
-  </si>
-  <si>
     <t>$\mathds{1}(\text{Def}_i)$</t>
   </si>
   <si>
-    <t>$\mathds{1}(\text{Def}_i)}\times \text{Val-Loan Dif}_i$</t>
+    <t>$\sum_t P^I_{it}$</t>
+  </si>
+  <si>
+    <t>$\sum_t P^F_{it}$</t>
+  </si>
+  <si>
+    <t>$\mathds{1}(\text{Def}_i)}\times\sum_t P^C_{it}$</t>
+  </si>
+  <si>
+    <t>$\mathds{1}(\text{Def}_i)}\times \text{Value-Loan}_i$</t>
   </si>
 </sst>
 </file>
@@ -736,22 +736,22 @@
   <dimension ref="A2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I13"/>
+      <selection activeCell="I13" sqref="A2:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="8" width="3.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="1"/>
+    <col min="8" max="8" width="3.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="11" t="s">
@@ -764,7 +764,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
@@ -787,26 +787,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="str">
         <f>[1]decomposition_main_te!A2</f>
         <v/>
@@ -841,7 +841,7 @@
         <v>(7)</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -874,7 +874,7 @@
         <v>-0.11***</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>[1]decomposition_main_te!A9</f>
         <v/>
@@ -908,7 +908,7 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -941,7 +941,7 @@
         <v>-0.0086</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="str">
         <f>[1]decomposition_main_te!B9</f>
         <v>(49.8)</v>
@@ -971,10 +971,10 @@
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>0.031</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0.57</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:G2"/>

</xml_diff>